<commit_message>
False alarm and detection time tables added.
</commit_message>
<xml_diff>
--- a/false_alarms.xlsx
+++ b/false_alarms.xlsx
@@ -95,7 +95,7 @@
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="11"/>
+        <sz val="28"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -112,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,8 +121,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <vertAlign val="superscript"/>
-      <sz val="11"/>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -178,55 +185,55 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,433 +623,441 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="7">
         <v>0.15</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="7">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="7">
         <v>0</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="8">
         <v>1.25</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="7">
         <v>0.1</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="8">
         <v>11.5</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="7">
         <v>0.12</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="7">
         <v>14.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="11">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="11">
         <v>0.1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="11">
         <v>0.1</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="12">
         <v>18.100000000000001</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="11">
         <v>1.6</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="12">
         <v>165.7</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="11">
         <v>1.9</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="11">
         <v>208.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10">
-        <v>100</v>
-      </c>
-      <c r="D6" s="10">
-        <v>100</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="C6" s="13">
+        <v>100</v>
+      </c>
+      <c r="D6" s="13">
+        <v>100</v>
+      </c>
+      <c r="E6" s="13">
         <v>1</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="13">
         <v>99.8</v>
       </c>
-      <c r="G6" s="10">
-        <v>100</v>
-      </c>
-      <c r="H6" s="10">
-        <v>100</v>
-      </c>
-      <c r="I6" s="10">
+      <c r="G6" s="13">
+        <v>100</v>
+      </c>
+      <c r="H6" s="13">
+        <v>100</v>
+      </c>
+      <c r="I6" s="13">
         <v>99.3</v>
       </c>
-      <c r="J6" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="11" t="s">
+      <c r="J6" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12">
-        <v>100</v>
-      </c>
-      <c r="D7" s="12">
-        <v>100</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="C7" s="16">
+        <v>100</v>
+      </c>
+      <c r="D7" s="16">
+        <v>100</v>
+      </c>
+      <c r="E7" s="16">
         <v>0</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="16">
         <v>97.7</v>
       </c>
-      <c r="G7" s="12">
-        <v>100</v>
-      </c>
-      <c r="H7" s="12">
-        <v>100</v>
-      </c>
-      <c r="I7" s="12">
-        <v>100</v>
-      </c>
-      <c r="J7" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="7" t="s">
+      <c r="G7" s="16">
+        <v>100</v>
+      </c>
+      <c r="H7" s="16">
+        <v>100</v>
+      </c>
+      <c r="I7" s="16">
+        <v>100</v>
+      </c>
+      <c r="J7" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13">
-        <v>100</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="C8" s="17">
+        <v>100</v>
+      </c>
+      <c r="D8" s="17">
         <v>32</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="17">
         <v>0</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="17">
         <v>96.5</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10">
-        <v>100</v>
-      </c>
-      <c r="D9" s="10">
-        <v>100</v>
-      </c>
-      <c r="E9" s="10">
+      <c r="C9" s="13">
+        <v>100</v>
+      </c>
+      <c r="D9" s="13">
+        <v>100</v>
+      </c>
+      <c r="E9" s="13">
         <v>0</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="13">
         <v>97.7</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="13">
         <v>25.8</v>
       </c>
-      <c r="H9" s="10">
-        <v>100</v>
-      </c>
-      <c r="I9" s="10">
+      <c r="H9" s="13">
+        <v>100</v>
+      </c>
+      <c r="I9" s="13">
         <v>20.3</v>
       </c>
-      <c r="J9" s="10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="11" t="s">
+      <c r="J9" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12">
-        <v>100</v>
-      </c>
-      <c r="D10" s="12">
-        <v>100</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="C10" s="16">
+        <v>100</v>
+      </c>
+      <c r="D10" s="16">
+        <v>100</v>
+      </c>
+      <c r="E10" s="16">
         <v>0</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="16">
         <v>7.7</v>
       </c>
-      <c r="G10" s="12">
-        <v>100</v>
-      </c>
-      <c r="H10" s="12">
-        <v>100</v>
-      </c>
-      <c r="I10" s="12">
-        <v>100</v>
-      </c>
-      <c r="J10" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="7" t="s">
+      <c r="G10" s="16">
+        <v>100</v>
+      </c>
+      <c r="H10" s="16">
+        <v>100</v>
+      </c>
+      <c r="I10" s="16">
+        <v>100</v>
+      </c>
+      <c r="J10" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="13">
-        <v>100</v>
-      </c>
-      <c r="D11" s="13">
-        <v>100</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="C11" s="17">
+        <v>100</v>
+      </c>
+      <c r="D11" s="17">
+        <v>100</v>
+      </c>
+      <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="17">
         <v>97</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10">
-        <v>100</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C12" s="13">
+        <v>100</v>
+      </c>
+      <c r="D12" s="13">
         <v>16.2</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="13">
         <v>3</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="13">
         <v>30.6</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="13">
         <v>92.9</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="13">
         <v>98.5</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="13">
         <v>93</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="13">
         <v>98.8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="11" t="s">
+    <row r="13" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="12">
-        <v>100</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="C13" s="16">
+        <v>100</v>
+      </c>
+      <c r="D13" s="16">
         <v>99.7</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="16">
         <v>98.3</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="16">
         <v>99</v>
       </c>
-      <c r="G13" s="12">
-        <v>100</v>
-      </c>
-      <c r="H13" s="12">
-        <v>100</v>
-      </c>
-      <c r="I13" s="12">
-        <v>100</v>
-      </c>
-      <c r="J13" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="7" t="s">
+      <c r="G13" s="16">
+        <v>100</v>
+      </c>
+      <c r="H13" s="16">
+        <v>100</v>
+      </c>
+      <c r="I13" s="16">
+        <v>100</v>
+      </c>
+      <c r="J13" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="13">
-        <v>100</v>
-      </c>
-      <c r="D14" s="13">
+      <c r="C14" s="17">
+        <v>100</v>
+      </c>
+      <c r="D14" s="17">
         <v>14</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="17">
         <v>0</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="17">
         <v>97</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="11" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:D8">
     <cfRule type="cellIs" dxfId="14" priority="30" operator="equal">

</xml_diff>